<commit_message>
Evaluations: #17 Part 1. CSS selectors by functions in AST.
</commit_message>
<xml_diff>
--- a/eval/e17/selectors.xlsx
+++ b/eval/e17/selectors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Selectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
   <si>
     <t>Site</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>1 Found</t>
   </si>
 </sst>
 </file>
@@ -568,9 +574,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -578,11 +584,12 @@
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="61.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,13 +609,16 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -630,8 +640,11 @@
       <c r="G2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
@@ -653,8 +666,11 @@
       <c r="G3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -676,8 +692,11 @@
       <c r="G4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>2</v>
       </c>
@@ -699,8 +718,11 @@
       <c r="G5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>2</v>
       </c>
@@ -722,8 +744,11 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>2</v>
       </c>
@@ -745,8 +770,11 @@
       <c r="G7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>2</v>
       </c>
@@ -768,8 +796,11 @@
       <c r="G8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>2</v>
       </c>
@@ -791,8 +822,11 @@
       <c r="G9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>2</v>
       </c>
@@ -814,8 +848,11 @@
       <c r="G10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>2</v>
       </c>
@@ -837,8 +874,11 @@
       <c r="G11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>2</v>
       </c>
@@ -860,8 +900,11 @@
       <c r="G12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>3</v>
       </c>
@@ -884,10 +927,13 @@
         <v>34</v>
       </c>
       <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>4</v>
       </c>
@@ -910,10 +956,13 @@
         <v>34</v>
       </c>
       <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>4</v>
       </c>
@@ -936,10 +985,13 @@
         <v>34</v>
       </c>
       <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>4</v>
       </c>
@@ -962,10 +1014,13 @@
         <v>34</v>
       </c>
       <c r="H16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>4</v>
       </c>
@@ -988,6 +1043,9 @@
         <v>34</v>
       </c>
       <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1004,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1039,6 +1097,14 @@
         <v>39</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Evaluations: #17 Complete.  Extracted selectors by all 3 methods.
</commit_message>
<xml_diff>
--- a/eval/e17/selectors.xlsx
+++ b/eval/e17/selectors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="40960" windowHeight="25140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Selectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="43">
   <si>
     <t>Site</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>2 Found</t>
   </si>
   <si>
     <t>title</t>
@@ -574,22 +577,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
-    <col min="9" max="9" width="61.6640625" customWidth="1"/>
+    <col min="7" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,16 +612,19 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -640,11 +646,11 @@
       <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -666,11 +672,11 @@
       <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
@@ -692,11 +698,11 @@
       <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>2</v>
       </c>
@@ -718,11 +724,11 @@
       <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>2</v>
       </c>
@@ -744,11 +750,11 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>2</v>
       </c>
@@ -770,11 +776,11 @@
       <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>2</v>
       </c>
@@ -796,11 +802,11 @@
       <c r="G8" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2</v>
       </c>
@@ -822,11 +828,11 @@
       <c r="G9" t="s">
         <v>34</v>
       </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>2</v>
       </c>
@@ -848,11 +854,11 @@
       <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>2</v>
       </c>
@@ -874,11 +880,11 @@
       <c r="G11" t="s">
         <v>34</v>
       </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>2</v>
       </c>
@@ -900,11 +906,11 @@
       <c r="G12" t="s">
         <v>34</v>
       </c>
-      <c r="H12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>3</v>
       </c>
@@ -926,14 +932,14 @@
       <c r="G13" t="s">
         <v>34</v>
       </c>
-      <c r="H13" t="s">
-        <v>34</v>
-      </c>
       <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>4</v>
       </c>
@@ -955,14 +961,14 @@
       <c r="G14" t="s">
         <v>34</v>
       </c>
-      <c r="H14" t="s">
-        <v>34</v>
-      </c>
       <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>4</v>
       </c>
@@ -984,14 +990,14 @@
       <c r="G15" t="s">
         <v>34</v>
       </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
       <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1013,14 +1019,14 @@
       <c r="G16" t="s">
         <v>34</v>
       </c>
-      <c r="H16" t="s">
-        <v>34</v>
-      </c>
       <c r="I16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1042,10 +1048,10 @@
       <c r="G17" t="s">
         <v>34</v>
       </c>
-      <c r="H17" t="s">
-        <v>34</v>
-      </c>
       <c r="I17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1102,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evaluations: #17, Extract selectors automatically from code blocks.
</commit_message>
<xml_diff>
--- a/eval/e17/selectors.xlsx
+++ b/eval/e17/selectors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="40960" windowHeight="25140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Selectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>Site</t>
   </si>
@@ -580,7 +580,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -646,6 +646,9 @@
       <c r="G2" t="s">
         <v>34</v>
       </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
       <c r="I2" t="s">
         <v>34</v>
       </c>
@@ -672,6 +675,9 @@
       <c r="G3" t="s">
         <v>34</v>
       </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
       <c r="I3" t="s">
         <v>34</v>
       </c>
@@ -698,6 +704,9 @@
       <c r="G4" t="s">
         <v>34</v>
       </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
       <c r="I4" t="s">
         <v>34</v>
       </c>
@@ -724,6 +733,9 @@
       <c r="G5" t="s">
         <v>34</v>
       </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
       <c r="I5" t="s">
         <v>34</v>
       </c>
@@ -750,6 +762,9 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
       <c r="I6" t="s">
         <v>34</v>
       </c>
@@ -776,6 +791,9 @@
       <c r="G7" t="s">
         <v>34</v>
       </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" t="s">
         <v>34</v>
       </c>
@@ -802,6 +820,9 @@
       <c r="G8" t="s">
         <v>34</v>
       </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
       <c r="I8" t="s">
         <v>34</v>
       </c>
@@ -828,6 +849,9 @@
       <c r="G9" t="s">
         <v>34</v>
       </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
       <c r="I9" t="s">
         <v>34</v>
       </c>
@@ -854,6 +878,9 @@
       <c r="G10" t="s">
         <v>34</v>
       </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" t="s">
         <v>34</v>
       </c>
@@ -880,6 +907,9 @@
       <c r="G11" t="s">
         <v>34</v>
       </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
       <c r="I11" t="s">
         <v>34</v>
       </c>
@@ -906,6 +936,9 @@
       <c r="G12" t="s">
         <v>34</v>
       </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
       <c r="I12" t="s">
         <v>34</v>
       </c>
@@ -932,6 +965,9 @@
       <c r="G13" t="s">
         <v>34</v>
       </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
       <c r="I13" t="s">
         <v>34</v>
       </c>
@@ -961,6 +997,9 @@
       <c r="G14" t="s">
         <v>34</v>
       </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
       <c r="I14" t="s">
         <v>34</v>
       </c>
@@ -990,6 +1029,9 @@
       <c r="G15" t="s">
         <v>34</v>
       </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" t="s">
         <v>34</v>
       </c>
@@ -1019,6 +1061,9 @@
       <c r="G16" t="s">
         <v>34</v>
       </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
       <c r="I16" t="s">
         <v>34</v>
       </c>
@@ -1046,6 +1091,9 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
         <v>34</v>
       </c>
       <c r="I17" t="s">

</xml_diff>